<commit_message>
Recomendacoes do delicious rotina para importar recomendacoes da omegashop
</commit_message>
<xml_diff>
--- a/poc.xlsx
+++ b/poc.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>Rose</t>
   </si>
@@ -67,6 +67,39 @@
   </si>
   <si>
     <t>Total/Sim. Sum</t>
+  </si>
+  <si>
+    <t>Itens recommendations for Tobby</t>
+  </si>
+  <si>
+    <t>Movie</t>
+  </si>
+  <si>
+    <t>Snakes</t>
+  </si>
+  <si>
+    <t>Superman</t>
+  </si>
+  <si>
+    <t>Dupree</t>
+  </si>
+  <si>
+    <t>Normalized</t>
+  </si>
+  <si>
+    <t>Rating</t>
+  </si>
+  <si>
+    <t>R.xNight</t>
+  </si>
+  <si>
+    <t>R.xLady</t>
+  </si>
+  <si>
+    <t>R.xLuck</t>
+  </si>
+  <si>
+    <t>Creating Recommendations for Toby</t>
   </si>
 </sst>
 </file>
@@ -74,9 +107,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -116,8 +149,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -142,8 +198,32 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor theme="8" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor theme="8" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -151,8 +231,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -162,11 +257,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -174,16 +273,37 @@
     <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
@@ -205,8 +325,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H9">
-  <autoFilter ref="A1:H9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:H10">
+  <autoFilter ref="A2:H10"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Critic" totalsRowLabel="Total"/>
     <tableColumn id="2" name="Similarity"/>
@@ -543,10 +663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="222" zoomScaleNormal="222" zoomScalePageLayoutView="222" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="222" zoomScaleNormal="222" zoomScalePageLayoutView="222" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -555,252 +675,444 @@
     <col min="2" max="2" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" t="s">
-        <v>12</v>
-      </c>
+    <row r="1" spans="1:8" ht="30">
+      <c r="A1" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>0.99</v>
-      </c>
-      <c r="C2" s="2">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1">
-        <f>B2*C2</f>
-        <v>2.9699999999999998</v>
-      </c>
-      <c r="E2" s="1">
-        <v>2.5</v>
-      </c>
-      <c r="F2" s="1">
-        <f>B2*E2</f>
-        <v>2.4750000000000001</v>
-      </c>
-      <c r="G2" s="1">
-        <v>3</v>
-      </c>
-      <c r="H2" s="1">
-        <f>B2*G2</f>
-        <v>2.9699999999999998</v>
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3">
-        <v>0.38</v>
+        <v>0.99</v>
       </c>
       <c r="C3" s="2">
         <v>3</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D6" si="0">B3*C3</f>
-        <v>1.1400000000000001</v>
+        <f>B3*C3</f>
+        <v>2.9699999999999998</v>
       </c>
       <c r="E3" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F3" s="1">
+        <f>B3*E3</f>
+        <v>2.4750000000000001</v>
+      </c>
+      <c r="G3" s="1">
         <v>3</v>
       </c>
-      <c r="F3" s="1">
-        <f t="shared" ref="F3:F6" si="1">B3*E3</f>
-        <v>1.1400000000000001</v>
-      </c>
-      <c r="G3" s="1">
-        <v>1.5</v>
-      </c>
       <c r="H3" s="1">
-        <f t="shared" ref="H3:H6" si="2">B3*G3</f>
-        <v>0.57000000000000006</v>
+        <f>B3*G3</f>
+        <v>2.9699999999999998</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>0.38</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" ref="D4:D7" si="0">B4*C4</f>
+        <v>1.1400000000000001</v>
+      </c>
+      <c r="E4" s="1">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" ref="F4:F7" si="1">B4*E4</f>
+        <v>1.1400000000000001</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" ref="H4:H7" si="2">B4*G4</f>
+        <v>0.57000000000000006</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>0.89</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C5" s="2">
         <v>4.5</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D5" s="1">
         <f t="shared" si="0"/>
         <v>4.0049999999999999</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1">
+      <c r="E5" s="1"/>
+      <c r="F5" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G5" s="1">
         <v>3</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H5" s="1">
         <f t="shared" si="2"/>
         <v>2.67</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="s">
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>0.92</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C6" s="2">
         <v>3</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D6" s="1">
         <f t="shared" si="0"/>
         <v>2.7600000000000002</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E6" s="1">
         <v>3</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F6" s="1">
         <f t="shared" si="1"/>
         <v>2.7600000000000002</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G6" s="1">
         <v>2</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H6" s="1">
         <f t="shared" si="2"/>
         <v>1.84</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>0.66</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C7" s="2">
         <v>3</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D7" s="1">
         <f t="shared" si="0"/>
         <v>1.98</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E7" s="1">
         <v>3</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F7" s="1">
         <f t="shared" si="1"/>
         <v>1.98</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1">
+      <c r="G7" s="1"/>
+      <c r="H7" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="3" t="s">
+    <row r="8" spans="1:8">
+      <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="7">
-        <f>SUM(B2:B6)</f>
+      <c r="B8" s="7">
+        <f>SUM(B3:B7)</f>
         <v>3.8400000000000003</v>
       </c>
-      <c r="C7" s="7">
-        <f>SUM(C2:C6)</f>
+      <c r="C8" s="7">
+        <f>SUM(C3:C7)</f>
         <v>16.5</v>
       </c>
-      <c r="D7" s="7">
-        <f>SUM(D2:D6)</f>
+      <c r="D8" s="7">
+        <f>SUM(D3:D7)</f>
         <v>12.854999999999999</v>
       </c>
-      <c r="E7" s="7">
-        <f>SUM(E2:E6)</f>
+      <c r="E8" s="7">
+        <f>SUM(E3:E7)</f>
         <v>11.5</v>
       </c>
-      <c r="F7" s="7">
-        <f>SUM(F2:F6)</f>
+      <c r="F8" s="7">
+        <f>SUM(F3:F7)</f>
         <v>8.3550000000000004</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G8" s="9">
         <v>12.86</v>
       </c>
-      <c r="H7" s="7">
-        <f>SUM(H2:H6)</f>
+      <c r="H8" s="7">
+        <f>SUM(H3:H7)</f>
         <v>8.0500000000000007</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="5" t="s">
+    <row r="9" spans="1:8">
+      <c r="A9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="8">
-        <f>SUM(B2:B6)</f>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="8">
+        <f>SUM(B3:B7)</f>
         <v>3.8400000000000003</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="8">
-        <f>B7-B4</f>
+      <c r="E9" s="6"/>
+      <c r="F9" s="8">
+        <f>B8-B5</f>
         <v>2.95</v>
       </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="8">
-        <f>B7-B6</f>
+      <c r="G9" s="6"/>
+      <c r="H9" s="8">
+        <f>B8-B7</f>
         <v>3.18</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="3" t="s">
+    <row r="10" spans="1:8">
+      <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="7">
-        <f>D7/B7</f>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="7">
+        <f>D8/B8</f>
         <v>3.3476562499999996</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="7">
-        <f>F7/F8</f>
+      <c r="E10" s="4"/>
+      <c r="F10" s="7">
+        <f>F8/F9</f>
         <v>2.8322033898305086</v>
       </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="7">
-        <f>H7/H8</f>
+      <c r="G10" s="4"/>
+      <c r="H10" s="7">
+        <f>H8/H9</f>
         <v>2.5314465408805034</v>
       </c>
     </row>
+    <row r="12" spans="1:8" ht="30">
+      <c r="A12" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="15">
+        <v>4.5</v>
+      </c>
+      <c r="C14" s="15">
+        <v>0.182</v>
+      </c>
+      <c r="D14" s="15">
+        <f>C14*B14</f>
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="E14" s="15">
+        <v>0.222</v>
+      </c>
+      <c r="F14" s="15">
+        <f>E14*B14</f>
+        <v>0.999</v>
+      </c>
+      <c r="G14" s="15">
+        <v>0.105</v>
+      </c>
+      <c r="H14" s="15">
+        <f>G14*B14</f>
+        <v>0.47249999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="17">
+        <v>4</v>
+      </c>
+      <c r="C15" s="17">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="D15" s="17">
+        <f t="shared" ref="D15:D16" si="3">C15*B15</f>
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="E15" s="17">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="F15" s="17">
+        <f t="shared" ref="F15:F16" si="4">E15*B15</f>
+        <v>0.36399999999999999</v>
+      </c>
+      <c r="G15" s="17">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="H15" s="17">
+        <f t="shared" ref="H15:H16" si="5">G15*B15</f>
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="15">
+        <v>1</v>
+      </c>
+      <c r="C16" s="15">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="D16" s="15">
+        <f t="shared" si="3"/>
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="E16" s="15">
+        <v>0.4</v>
+      </c>
+      <c r="F16" s="15">
+        <f t="shared" si="4"/>
+        <v>0.4</v>
+      </c>
+      <c r="G16" s="15">
+        <v>0.182</v>
+      </c>
+      <c r="H16" s="15">
+        <f t="shared" si="5"/>
+        <v>0.182</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19">
+        <f>SUM(C14:C16)</f>
+        <v>0.43299999999999994</v>
+      </c>
+      <c r="D17" s="19">
+        <f>SUM(D14:D16)</f>
+        <v>1.3789999999999998</v>
+      </c>
+      <c r="E17" s="19">
+        <f t="shared" ref="E17:H17" si="6">SUM(E14:E16)</f>
+        <v>0.71300000000000008</v>
+      </c>
+      <c r="F17" s="19">
+        <f t="shared" si="6"/>
+        <v>1.7629999999999999</v>
+      </c>
+      <c r="G17" s="20">
+        <f t="shared" si="6"/>
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="H17" s="19">
+        <f t="shared" si="6"/>
+        <v>0.91449999999999987</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="22">
+        <f>D17/C17</f>
+        <v>3.1847575057736721</v>
+      </c>
+      <c r="E18" s="21"/>
+      <c r="F18" s="22">
+        <f>F17/E17</f>
+        <v>2.4726507713884991</v>
+      </c>
+      <c r="G18" s="21"/>
+      <c r="H18" s="22">
+        <f>H17/G17</f>
+        <v>2.5980113636363633</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A12:H12"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <ignoredErrors>
-    <ignoredError sqref="F4" emptyCellReference="1"/>
+    <ignoredError sqref="F5" emptyCellReference="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>